<commit_message>
avances con practica de ISO
</commit_message>
<xml_diff>
--- a/2do/ISO/Practica2/Scheduling.xlsx
+++ b/2do/ISO/Practica2/Scheduling.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="47">
   <si>
     <t>Proceso</t>
   </si>
@@ -112,6 +113,60 @@
   <si>
     <t>RR Q=6</t>
   </si>
+  <si>
+    <t>I/O (rec, ins, dur)</t>
+  </si>
+  <si>
+    <t>(R1, 4, 2) (R2, 6, 3) (R1, 8, 3)</t>
+  </si>
+  <si>
+    <t>(R3, 3, 2) (R3, 4, 2)</t>
+  </si>
+  <si>
+    <t>(R1, 4, 1)</t>
+  </si>
+  <si>
+    <t>(R2, 1, 2) (R2, 5, 3)</t>
+  </si>
+  <si>
+    <t>(R1, 2, 3) (R3, 4, 3)</t>
+  </si>
+  <si>
+    <t>Queu</t>
+  </si>
+  <si>
+    <t>Queu R1</t>
+  </si>
+  <si>
+    <t>Queu R2</t>
+  </si>
+  <si>
+    <t>Queu R3</t>
+  </si>
+  <si>
+    <t>I/O FCFS</t>
+  </si>
+  <si>
+    <t>RR Q=3</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Queu P1</t>
+  </si>
+  <si>
+    <t>Queu P2</t>
+  </si>
+  <si>
+    <t>Queu P3</t>
+  </si>
 </sst>
 </file>
 
@@ -142,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -176,11 +231,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -188,6 +278,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5668,4 +5761,1112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="36" width="5.5546875" customWidth="1"/>
+    <col min="37" max="37" width="5.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E7" s="7"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>6</v>
+      </c>
+      <c r="M7" s="1">
+        <v>7</v>
+      </c>
+      <c r="N7" s="1">
+        <v>8</v>
+      </c>
+      <c r="O7" s="1">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>11</v>
+      </c>
+      <c r="R7" s="1">
+        <v>12</v>
+      </c>
+      <c r="S7" s="1">
+        <v>13</v>
+      </c>
+      <c r="T7" s="1">
+        <v>14</v>
+      </c>
+      <c r="U7" s="1">
+        <v>15</v>
+      </c>
+      <c r="V7" s="1">
+        <v>16</v>
+      </c>
+      <c r="W7" s="1">
+        <v>17</v>
+      </c>
+      <c r="X7" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>22</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>24</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>25</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>26</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>28</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>29</v>
+      </c>
+      <c r="AJ7" s="8">
+        <v>30</v>
+      </c>
+      <c r="AK7" s="9"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E8" s="7"/>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
+        <v>4</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1">
+        <v>5</v>
+      </c>
+      <c r="V8" s="1">
+        <v>6</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK8" s="9"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E9" s="7"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1">
+        <v>4</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="9"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1">
+        <v>4</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="9"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1">
+        <v>2</v>
+      </c>
+      <c r="X11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="9"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E12" s="7"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>2</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="9"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5">
+        <v>4</v>
+      </c>
+      <c r="K13" s="5">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5">
+        <v>2</v>
+      </c>
+      <c r="M13" s="5">
+        <v>3</v>
+      </c>
+      <c r="N13" s="5">
+        <v>1</v>
+      </c>
+      <c r="O13" s="5">
+        <v>4</v>
+      </c>
+      <c r="P13" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>2</v>
+      </c>
+      <c r="R13" s="5">
+        <v>3</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="5">
+        <v>1</v>
+      </c>
+      <c r="U13" s="5">
+        <v>4</v>
+      </c>
+      <c r="V13" s="5">
+        <v>5</v>
+      </c>
+      <c r="W13" s="5">
+        <v>1</v>
+      </c>
+      <c r="X13" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="9"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+    </row>
+    <row r="17" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+    </row>
+    <row r="18" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E18" s="7"/>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>4</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5</v>
+      </c>
+      <c r="L18" s="1">
+        <v>6</v>
+      </c>
+      <c r="M18" s="1">
+        <v>7</v>
+      </c>
+      <c r="N18" s="1">
+        <v>8</v>
+      </c>
+      <c r="O18" s="1">
+        <v>9</v>
+      </c>
+      <c r="P18" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>11</v>
+      </c>
+      <c r="R18" s="1">
+        <v>12</v>
+      </c>
+      <c r="S18" s="1">
+        <v>13</v>
+      </c>
+      <c r="T18" s="1">
+        <v>14</v>
+      </c>
+      <c r="U18" s="1">
+        <v>15</v>
+      </c>
+      <c r="V18" s="1">
+        <v>16</v>
+      </c>
+      <c r="W18" s="1">
+        <v>17</v>
+      </c>
+      <c r="X18" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>19</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>22</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>24</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>25</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>26</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>28</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>29</v>
+      </c>
+      <c r="AJ18" s="8">
+        <v>30</v>
+      </c>
+      <c r="AK18" s="9"/>
+    </row>
+    <row r="19" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E19" s="7"/>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5</v>
+      </c>
+      <c r="M19" s="3">
+        <v>6</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>7</v>
+      </c>
+      <c r="R19" s="1">
+        <v>8</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="9"/>
+    </row>
+    <row r="20" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E20" s="7"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1">
+        <v>4</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="9"/>
+    </row>
+    <row r="21" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E21" s="7"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK21" s="9"/>
+    </row>
+    <row r="22" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E22" s="7"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="9"/>
+    </row>
+    <row r="23" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E23" s="7"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S23" s="1">
+        <v>3</v>
+      </c>
+      <c r="T23" s="1">
+        <v>4</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="9"/>
+    </row>
+    <row r="24" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>5</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
+      <c r="K24" s="5">
+        <v>5</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
+      <c r="G25" s="5">
+        <v>4</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2</v>
+      </c>
+      <c r="I25" s="5">
+        <v>4</v>
+      </c>
+      <c r="J25" s="5">
+        <v>2</v>
+      </c>
+      <c r="K25" s="5">
+        <v>4</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="5:37" x14ac:dyDescent="0.3">
+      <c r="E26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="5">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>